<commit_message>
read and write data
</commit_message>
<xml_diff>
--- a/cypress/fixtures/user.xlsx
+++ b/cypress/fixtures/user.xlsx
@@ -415,24 +415,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Kendra Rempel-Swaniawski</v>
+        <v>Teresa Rolfson</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" t="str">
-        <v>Edgar35@yahoo.com</v>
+        <v>Ansley_Marvin77@hotmail.com</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Ernestine Gulgowski</v>
+        <v>Gregg Hyatt III</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C3" t="str">
-        <v>Mark58@yahoo.com</v>
+        <v>Marta.Schulist@yahoo.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>